<commit_message>
Graph working (but no visibility control yet)
</commit_message>
<xml_diff>
--- a/docs/RDUcommands.xlsx
+++ b/docs/RDUcommands.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="48" windowWidth="18072" windowHeight="10188"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="18072" windowHeight="10188" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Protocol" sheetId="1" r:id="rId1"/>
+    <sheet name="Specs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="164">
   <si>
     <t>DA</t>
   </si>
@@ -583,12 +582,168 @@
   <si>
     <t>Ambient T*10, C (may be negative!)</t>
   </si>
+  <si>
+    <t>Max Input Voltage</t>
+  </si>
+  <si>
+    <t>Max Current 5 seconds*</t>
+  </si>
+  <si>
+    <t>300 A</t>
+  </si>
+  <si>
+    <t>Max Current 30 seconds*</t>
+  </si>
+  <si>
+    <t>150 A</t>
+  </si>
+  <si>
+    <t>Max Continuous Current*</t>
+  </si>
+  <si>
+    <t>75 A</t>
+  </si>
+  <si>
+    <t>Shunt Resistance</t>
+  </si>
+  <si>
+    <t>0.0002 Ω</t>
+  </si>
+  <si>
+    <t>Internal Resolution V</t>
+  </si>
+  <si>
+    <t>0.001 V</t>
+  </si>
+  <si>
+    <t>Displayed Resolution V</t>
+  </si>
+  <si>
+    <t>0.01 V</t>
+  </si>
+  <si>
+    <t>Internal Resolution A</t>
+  </si>
+  <si>
+    <t>0.04 A</t>
+  </si>
+  <si>
+    <t>Displayed Resolution A</t>
+  </si>
+  <si>
+    <t>0.1 A</t>
+  </si>
+  <si>
+    <t>TMP Sensor Resolution</t>
+  </si>
+  <si>
+    <t>0.1 C</t>
+  </si>
+  <si>
+    <t>TMP Sensor Accuracy</t>
+  </si>
+  <si>
+    <t>Analog&lt;&gt;Digital Converters</t>
+  </si>
+  <si>
+    <t>16 bit</t>
+  </si>
+  <si>
+    <t>Phase RPM Max Readable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RDU (from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Emeter2 Quick Guide 2.09</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase RPM Resolution (14 mag motor)</t>
+  </si>
+  <si>
+    <t>17 rpm</t>
+  </si>
+  <si>
+    <t>MDU</t>
+  </si>
+  <si>
+    <t>35 V</t>
+  </si>
+  <si>
+    <t>70 V</t>
+  </si>
+  <si>
+    <t>25 A</t>
+  </si>
+  <si>
+    <t>50 A</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>13 g</t>
+  </si>
+  <si>
+    <t>20 x 17 x 15</t>
+  </si>
+  <si>
+    <t>Dimensions, mm</t>
+  </si>
+  <si>
+    <t>36 x 29 x 13.5</t>
+  </si>
+  <si>
+    <t>28 g</t>
+  </si>
+  <si>
+    <t>LDU</t>
+  </si>
+  <si>
+    <t>24 g</t>
+  </si>
+  <si>
+    <t>31 x 26 x 13.4</t>
+  </si>
+  <si>
+    <t>On-board memory/samples</t>
+  </si>
+  <si>
+    <t>128 KB/5000</t>
+  </si>
+  <si>
+    <t>64 KB/2500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +768,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -669,6 +843,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -1281,7 +1473,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1654,24 +1846,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="12">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed discharge calculation; cleared COM cache on connection; minor UI improvements
</commit_message>
<xml_diff>
--- a/docs/RDUcommands.xlsx
+++ b/docs/RDUcommands.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="165">
   <si>
     <t>DA</t>
   </si>
@@ -623,9 +623,6 @@
   </si>
   <si>
     <t>Internal Resolution A</t>
-  </si>
-  <si>
-    <t>0.04 A</t>
   </si>
   <si>
     <t>Displayed Resolution A</t>
@@ -738,12 +735,41 @@
   <si>
     <t>64 KB/2500</t>
   </si>
+  <si>
+    <t>0.04A  (1st @ 220mA)</t>
+  </si>
+  <si>
+    <r>
+      <t>0.02A (1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @ 120mA)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,6 +820,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -836,13 +870,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -855,6 +882,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1207,13 +1241,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
@@ -1221,9 +1255,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1232,9 +1266,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1243,9 +1277,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1254,9 +1288,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1265,9 +1299,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
@@ -1276,9 +1310,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1287,9 +1321,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="6" t="s">
         <v>15</v>
       </c>
@@ -1298,9 +1332,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1309,9 +1343,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1320,9 +1354,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1331,9 +1365,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="6" t="s">
         <v>22</v>
       </c>
@@ -1342,9 +1376,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1353,9 +1387,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="7" t="s">
         <v>25</v>
       </c>
@@ -1364,9 +1398,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" t="s">
         <v>26</v>
       </c>
@@ -1375,9 +1409,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" t="s">
         <v>27</v>
       </c>
@@ -1386,9 +1420,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
       <c r="D23" t="s">
         <v>28</v>
       </c>
@@ -1397,9 +1431,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
       <c r="D24" t="s">
         <v>29</v>
       </c>
@@ -1408,9 +1442,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" t="s">
         <v>30</v>
       </c>
@@ -1419,9 +1453,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
       <c r="D26" t="s">
         <v>35</v>
       </c>
@@ -1430,9 +1464,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
       <c r="D27" t="s">
         <v>36</v>
       </c>
@@ -1441,9 +1475,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1452,9 +1486,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="1" t="s">
         <v>38</v>
       </c>
@@ -1463,9 +1497,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="2">
         <v>44</v>
       </c>
@@ -1580,13 +1614,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D39" s="2">
@@ -1597,18 +1631,18 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="2"/>
       <c r="E40" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="2">
         <v>1</v>
       </c>
@@ -1617,9 +1651,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="2" t="s">
         <v>5</v>
       </c>
@@ -1628,9 +1662,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
@@ -1639,9 +1673,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="2">
         <v>6</v>
       </c>
@@ -1650,9 +1684,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="2">
         <v>7</v>
       </c>
@@ -1661,9 +1695,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="2">
         <v>8</v>
       </c>
@@ -1672,9 +1706,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="2">
         <v>9</v>
       </c>
@@ -1734,17 +1768,17 @@
       <c r="C51" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -1761,13 +1795,13 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D53" t="s">
@@ -1778,9 +1812,9 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
       <c r="D54" t="s">
         <v>105</v>
       </c>
@@ -1789,9 +1823,9 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
       <c r="D55" t="s">
         <v>96</v>
       </c>
@@ -1800,14 +1834,14 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
       <c r="D57" t="s">
         <v>95</v>
       </c>
@@ -1816,9 +1850,9 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
       <c r="D58" t="s">
         <v>100</v>
       </c>
@@ -1849,41 +1883,41 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>158</v>
+      <c r="A1" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
         <v>161</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>162</v>
       </c>
-      <c r="C3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1892,10 +1926,10 @@
         <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1906,7 +1940,7 @@
         <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1925,7 +1959,7 @@
         <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1952,88 +1986,91 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
         <v>136</v>
-      </c>
-      <c r="B12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
         <v>138</v>
-      </c>
-      <c r="B13" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="11">
+        <v>139</v>
+      </c>
+      <c r="B14" s="8">
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
         <v>141</v>
-      </c>
-      <c r="B15" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="12">
+        <v>142</v>
+      </c>
+      <c r="B16" s="9">
         <v>65000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
         <v>145</v>
-      </c>
-      <c r="B17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" t="s">
         <v>155</v>
       </c>
-      <c r="B18" t="s">
-        <v>156</v>
-      </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
       </c>
-      <c r="B19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" t="s">
-        <v>153</v>
-      </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>